<commit_message>
Updates to rental and video
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogda\Code\GitHub\risestudiosbk\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED415DA-801E-4BBA-80D8-0055815DE1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9878827-54F3-411A-AFB8-575F041AE93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{3C06EA01-D4D4-4253-A5C0-9A16AF6880E1}"/>
+    <workbookView xWindow="-15030" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3C06EA01-D4D4-4253-A5C0-9A16AF6880E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>Description</t>
   </si>
@@ -202,10 +202,103 @@
     <t>Accessories</t>
   </si>
   <si>
-    <t>Blackout Dates</t>
-  </si>
-  <si>
-    <t>Weekdays</t>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Note: Checkbox means the time slot is not avaliable</t>
+  </si>
+  <si>
+    <t>10:00 AM - 11:00 AM</t>
+  </si>
+  <si>
+    <t>11:00 AM - 12:00 PM</t>
+  </si>
+  <si>
+    <t>10:00 PM - 11:00 PM</t>
+  </si>
+  <si>
+    <t>11:00 PM - 12:00 AM</t>
+  </si>
+  <si>
+    <t>01:00 AM - 02:00 AM</t>
+  </si>
+  <si>
+    <t>12:00 AM - 01:00 AM</t>
+  </si>
+  <si>
+    <t>02:00 AM - 03:00 AM</t>
+  </si>
+  <si>
+    <t>03:00 AM - 04:00 AM</t>
+  </si>
+  <si>
+    <t>04:00 AM - 05:00 AM</t>
+  </si>
+  <si>
+    <t>05:00 AM - 06:00 AM</t>
+  </si>
+  <si>
+    <t>06:00 AM - 07:00 AM</t>
+  </si>
+  <si>
+    <t>07:00 AM - 08:00 AM</t>
+  </si>
+  <si>
+    <t>08:00 AM - 09:00 AM</t>
+  </si>
+  <si>
+    <t>09:00 AM - 10:00 AM</t>
+  </si>
+  <si>
+    <t>12:00 PM - 01:00 PM</t>
+  </si>
+  <si>
+    <t>01:00 PM - 02:00 PM</t>
+  </si>
+  <si>
+    <t>02:00 PM - 03:00 PM</t>
+  </si>
+  <si>
+    <t>03:00 PM - 04:00 PM</t>
+  </si>
+  <si>
+    <t>04:00 PM - 05:00 PM</t>
+  </si>
+  <si>
+    <t>05:00 PM - 06:00 PM</t>
+  </si>
+  <si>
+    <t>06:00 PM - 07:00 PM</t>
+  </si>
+  <si>
+    <t>07:00 PM - 08:00 PM</t>
+  </si>
+  <si>
+    <t>08:00 PM - 09:00 PM</t>
+  </si>
+  <si>
+    <t>09:00 PM - 10:00 PM</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -261,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,11 +375,64 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="25">
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -465,46 +611,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{211927BF-93C8-4674-9DA1-7E6C553530A1}" name="Events" displayName="Events" ref="A1:F100" tableType="queryTable" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{211927BF-93C8-4674-9DA1-7E6C553530A1}" name="Events" displayName="Events" ref="A1:F100" tableType="queryTable" headerRowDxfId="24">
   <autoFilter ref="A1:F100" xr:uid="{211927BF-93C8-4674-9DA1-7E6C553530A1}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{B25BC987-858D-4556-A0E2-FE3B6F3F9E8E}" uniqueName="2" name="Title" totalsRowLabel="Total" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1D19D0F7-1E25-430B-BFC6-6A989435C904}" uniqueName="3" name="Date" queryTableFieldId="3" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{3F709EE1-4642-4316-ABDA-4567FA9C415C}" uniqueName="4" name="Location" queryTableFieldId="4" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{DC452608-C775-412C-9DEB-16AEC9490CDF}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{0D50D608-2536-4B14-9BE8-35EAA4E4203A}" uniqueName="7" name="Location Link" queryTableFieldId="7" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{7F9C7D3E-6B4B-4EA0-84C1-0CE97972BF4F}" uniqueName="8" name="Image Name" totalsRowFunction="count" queryTableFieldId="8" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B25BC987-858D-4556-A0E2-FE3B6F3F9E8E}" uniqueName="2" name="Title" totalsRowLabel="Total" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{1D19D0F7-1E25-430B-BFC6-6A989435C904}" uniqueName="3" name="Date" queryTableFieldId="3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{3F709EE1-4642-4316-ABDA-4567FA9C415C}" uniqueName="4" name="Location" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{DC452608-C775-412C-9DEB-16AEC9490CDF}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{0D50D608-2536-4B14-9BE8-35EAA4E4203A}" uniqueName="7" name="Location Link" queryTableFieldId="7" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{7F9C7D3E-6B4B-4EA0-84C1-0CE97972BF4F}" uniqueName="8" name="Image Name" totalsRowFunction="count" queryTableFieldId="8" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3186DF0F-4997-4830-83E0-6C7F5EBEF08E}" name="Shop" displayName="Shop" ref="A1:K9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3186DF0F-4997-4830-83E0-6C7F5EBEF08E}" name="Shop" displayName="Shop" ref="A1:K9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:K9" xr:uid="{3186DF0F-4997-4830-83E0-6C7F5EBEF08E}"/>
   <tableColumns count="11">
     <tableColumn id="4" xr3:uid="{4D35B921-12CB-441F-9702-7D6EFC37AC28}" uniqueName="4" name="ID" queryTableFieldId="6"/>
-    <tableColumn id="1" xr3:uid="{8778EBD2-B1EA-41B5-8833-9C54227B46BD}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{8778EBD2-B1EA-41B5-8833-9C54227B46BD}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{515F4FE7-5587-48FE-82DC-21CB1C57F023}" uniqueName="2" name="Price" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{E9F7001B-88D4-4FE3-B2D2-238BAB6377C6}" uniqueName="3" name="Category" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{36C927AF-D80C-4F77-80B4-2BC0CD2EC022}" uniqueName="5" name="Image Name" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{9AEC5D45-5308-47F8-A84F-D90C460AEFF5}" uniqueName="6" name="XS" queryTableFieldId="7" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{FFF459B7-C45F-42E3-935D-5F93E56ED28E}" uniqueName="7" name="S" queryTableFieldId="8" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{52AE7F97-C619-49FE-A626-6A60B135ECC6}" uniqueName="8" name="M" queryTableFieldId="9" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{4057B97A-9601-4D82-A2D4-508CD6130D5B}" uniqueName="9" name="L" queryTableFieldId="10" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{8AFDEE49-F78E-4EC9-AD60-4C5B7538F71D}" uniqueName="10" name="XL" queryTableFieldId="11" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{F8BC8748-E3E7-4BE8-8840-A4E2C80F5C23}" uniqueName="11" name="XXL" queryTableFieldId="12" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E9F7001B-88D4-4FE3-B2D2-238BAB6377C6}" uniqueName="3" name="Category" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{36C927AF-D80C-4F77-80B4-2BC0CD2EC022}" uniqueName="5" name="Image Name" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{9AEC5D45-5308-47F8-A84F-D90C460AEFF5}" uniqueName="6" name="XS" queryTableFieldId="7" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{FFF459B7-C45F-42E3-935D-5F93E56ED28E}" uniqueName="7" name="S" queryTableFieldId="8" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{52AE7F97-C619-49FE-A626-6A60B135ECC6}" uniqueName="8" name="M" queryTableFieldId="9" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{4057B97A-9601-4D82-A2D4-508CD6130D5B}" uniqueName="9" name="L" queryTableFieldId="10" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{8AFDEE49-F78E-4EC9-AD60-4C5B7538F71D}" uniqueName="10" name="XL" queryTableFieldId="11" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{F8BC8748-E3E7-4BE8-8840-A4E2C80F5C23}" uniqueName="11" name="XXL" queryTableFieldId="12" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E95D8D59-0AA2-4858-827B-CD105554B6F9}" name="Rentals" displayName="Rentals" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{E95D8D59-0AA2-4858-827B-CD105554B6F9}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DA552635-900E-4802-8032-B216DFA196AA}" name="Blackout Dates" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{0F2BAC03-F801-4D98-9F08-F7E499A8D2D8}" name="Weekdays"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E95D8D59-0AA2-4858-827B-CD105554B6F9}" name="Rentals" displayName="Rentals" ref="A1:H25" totalsRowShown="0">
+  <autoFilter ref="A1:H25" xr:uid="{E95D8D59-0AA2-4858-827B-CD105554B6F9}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DA552635-900E-4802-8032-B216DFA196AA}" name="Time" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0F2BAC03-F801-4D98-9F08-F7E499A8D2D8}" name="Sunday" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{76A062B5-61A2-41F9-9757-E30A57B15256}" name="Monday" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3B89D1F8-7E27-4C8F-9672-8AD0408DC9A7}" name="Tuesday" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{64C8B363-4C50-4425-A320-3ED5E57756A1}" name="Wednesday" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{948D81A7-42CE-4FA6-9694-3BB1C0DEA733}" name="Thursday" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{956FAA30-35B5-4A40-A21D-5D27F6F6E29E}" name="Friday" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{3DD3FDCB-5149-4F0F-90A4-CEA7CD004FA9}" name="Saturday" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1589,59 +1741,689 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E526ACF3-F34C-4FBB-86F4-190DDE192BFF}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>40959</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>40959</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A26:H26"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>